<commit_message>
Allow empty cell for not new NCBI taxa, construct_bi_or_tri emits ERROR not CRITICAL logs on failure, test file updates
</commit_message>
<xml_diff>
--- a/test/fixtures/Test_format_bad_NCBI.xlsx
+++ b/test/fixtures/Test_format_bad_NCBI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jc2017/Documents/MyRepos/safedata_validator/test/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dorme/Research/SAFE/Database/safedata_validator_package/test/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC599BC2-13C4-B243-A9BA-B476648EDD47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1099F0E7-9748-F242-9D20-66F9BB80EBEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27860" windowHeight="15840" activeTab="3" xr2:uid="{819B57D8-7F20-471A-9405-EB60A28E68AA}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="27860" windowHeight="15840" activeTab="4" xr2:uid="{819B57D8-7F20-471A-9405-EB60A28E68AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -2198,7 +2198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA5DB6CA-35DF-6D4E-8898-AF5D17F73D64}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -2470,8 +2470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6973E772-319E-4D19-B398-4AADD9788389}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="A1:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>